<commit_message>
for obi and dejan
Former-commit-id: c48ffe06d1627333882e091e69a4235d2887df83
</commit_message>
<xml_diff>
--- a/db/dummydata/ez_local_charges.xlsx
+++ b/db/dummydata/ez_local_charges.xlsx
@@ -25,7 +25,7 @@
     <t>DESTINATION</t>
   </si>
   <si>
-    <t>SERVICE LEVEL</t>
+    <t>SERVICE_LEVEL</t>
   </si>
   <si>
     <t>FEE</t>
@@ -85,9 +85,6 @@
     <t>Terminal Charge</t>
   </si>
   <si>
-    <t>rail</t>
-  </si>
-  <si>
     <t>ocean</t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>PER_CBM_TON</t>
+  </si>
+  <si>
+    <t>rail</t>
   </si>
   <si>
     <t>Customs Clearance</t>
@@ -179,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -188,6 +188,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -241,7 +244,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -289,7 +292,7 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
@@ -300,34 +303,34 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <f t="shared" ref="A2:A9" si="1">TODAY()</f>
-        <v>43263</v>
-      </c>
-      <c r="B2" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B2" s="5">
         <f t="shared" ref="B2:B9" si="2">A2 + 365</f>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L2" s="1">
         <v>150.0</v>
@@ -340,31 +343,31 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B3" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B3" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
       </c>
       <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="K3" t="s">
         <v>32</v>
@@ -374,31 +377,31 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B4" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B4" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
       </c>
       <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>32</v>
@@ -410,13 +413,13 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B5" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B5" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -424,16 +427,16 @@
         <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J5" t="s">
         <v>38</v>
@@ -449,34 +452,34 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B6" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B6" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
       </c>
       <c r="I6" t="s">
         <v>40</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L6" s="1">
         <v>150.0</v>
@@ -489,31 +492,31 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B7" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B7" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
         <v>40</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7" t="s">
         <v>32</v>
@@ -523,31 +526,31 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B8" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B8" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
         <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" t="s">
         <v>40</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>32</v>
@@ -559,13 +562,13 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="4">
+      <c r="A9" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B9" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B9" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -573,13 +576,13 @@
         <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" t="s">
         <v>40</v>
@@ -1616,7 +1619,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1664,7 +1667,7 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
@@ -1675,34 +1678,34 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <f t="shared" ref="A2:A9" si="1">TODAY()</f>
-        <v>43263</v>
-      </c>
-      <c r="B2" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B2" s="5">
         <f t="shared" ref="B2:B9" si="2">A2 + 365</f>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L2" s="1">
         <v>150.0</v>
@@ -1715,31 +1718,31 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B3" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B3" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
       </c>
       <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="K3" t="s">
         <v>32</v>
@@ -1749,31 +1752,31 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B4" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B4" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
       </c>
       <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>32</v>
@@ -1785,13 +1788,13 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B5" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B5" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1799,16 +1802,16 @@
         <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J5" t="s">
         <v>38</v>
@@ -1824,34 +1827,34 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B6" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B6" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
         <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
       </c>
       <c r="I6" t="s">
         <v>40</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L6" s="1">
         <v>150.0</v>
@@ -1864,31 +1867,31 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B7" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B7" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
         <v>40</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K7" t="s">
         <v>32</v>
@@ -1898,31 +1901,31 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B8" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B8" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
         <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" t="s">
         <v>40</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>32</v>
@@ -1934,13 +1937,13 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="4">
+      <c r="A9" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B9" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B9" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1948,13 +1951,13 @@
         <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" t="s">
         <v>40</v>
@@ -2991,7 +2994,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -3039,7 +3042,7 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
@@ -3050,39 +3053,39 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <f t="shared" ref="A2:A9" si="1">TODAY()</f>
-        <v>43263</v>
-      </c>
-      <c r="B2" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B2" s="5">
         <f t="shared" ref="B2:B9" si="2">A2 + 365</f>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="5">
+        <v>28</v>
+      </c>
+      <c r="L2" s="6">
         <v>18.75</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="6">
         <v>9.375</v>
       </c>
       <c r="N2">
@@ -3100,7 +3103,7 @@
       <c r="R2">
         <v>0.0</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="6">
         <v>18.75</v>
       </c>
       <c r="T2">
@@ -3108,28 +3111,28 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B3" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B3" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
       </c>
       <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>33</v>
@@ -3149,7 +3152,7 @@
       <c r="O3">
         <v>0.0</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="6">
         <v>31.25</v>
       </c>
       <c r="Q3">
@@ -3166,28 +3169,28 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B4" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B4" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
       </c>
       <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>33</v>
@@ -3195,7 +3198,7 @@
       <c r="K4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="6">
         <v>0.0</v>
       </c>
       <c r="M4">
@@ -3207,7 +3210,7 @@
       <c r="O4">
         <v>0.0</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="6">
         <v>31.25</v>
       </c>
       <c r="Q4">
@@ -3216,7 +3219,7 @@
       <c r="R4">
         <v>0.0</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4" s="6">
         <v>0.0</v>
       </c>
       <c r="T4">
@@ -3224,13 +3227,13 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B5" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B5" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -3238,16 +3241,16 @@
         <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>33</v>
@@ -3255,7 +3258,7 @@
       <c r="K5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="6">
         <v>20.75</v>
       </c>
       <c r="M5">
@@ -3276,7 +3279,7 @@
       <c r="R5">
         <v>0.0</v>
       </c>
-      <c r="S5" s="5">
+      <c r="S5" s="6">
         <v>20.75</v>
       </c>
       <c r="T5">
@@ -3284,25 +3287,25 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B6" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B6" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
         <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
       </c>
       <c r="I6" t="s">
         <v>40</v>
@@ -3311,12 +3314,12 @@
         <v>33</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="5">
+        <v>28</v>
+      </c>
+      <c r="L6" s="6">
         <v>18.75</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="6">
         <v>9.375</v>
       </c>
       <c r="N6">
@@ -3334,7 +3337,7 @@
       <c r="R6">
         <v>0.0</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S6" s="6">
         <v>18.75</v>
       </c>
       <c r="T6">
@@ -3342,25 +3345,25 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B7" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B7" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
         <v>40</v>
@@ -3383,7 +3386,7 @@
       <c r="O7">
         <v>0.0</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="6">
         <v>31.25</v>
       </c>
       <c r="Q7">
@@ -3400,25 +3403,25 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B8" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B8" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
         <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" t="s">
         <v>40</v>
@@ -3429,7 +3432,7 @@
       <c r="K8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="6">
         <v>0.0</v>
       </c>
       <c r="M8">
@@ -3441,7 +3444,7 @@
       <c r="O8">
         <v>0.0</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="6">
         <v>31.25</v>
       </c>
       <c r="Q8">
@@ -3450,7 +3453,7 @@
       <c r="R8">
         <v>0.0</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="6">
         <v>0.0</v>
       </c>
       <c r="T8">
@@ -3458,13 +3461,13 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="4">
+      <c r="A9" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B9" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B9" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -3472,13 +3475,13 @@
         <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" t="s">
         <v>40</v>
@@ -3489,7 +3492,7 @@
       <c r="K9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="6">
         <v>20.75</v>
       </c>
       <c r="M9">
@@ -3510,7 +3513,7 @@
       <c r="R9">
         <v>0.0</v>
       </c>
-      <c r="S9" s="5">
+      <c r="S9" s="6">
         <v>20.75</v>
       </c>
       <c r="T9">
@@ -4536,7 +4539,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -4584,7 +4587,7 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
@@ -4595,39 +4598,39 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <f t="shared" ref="A2:A9" si="1">TODAY()</f>
-        <v>43263</v>
-      </c>
-      <c r="B2" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B2" s="5">
         <f t="shared" ref="B2:B9" si="2">A2 + 365</f>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="5">
+        <v>28</v>
+      </c>
+      <c r="L2" s="6">
         <v>18.75</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="6">
         <v>9.375</v>
       </c>
       <c r="N2">
@@ -4645,7 +4648,7 @@
       <c r="R2">
         <v>0.0</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="6">
         <v>18.75</v>
       </c>
       <c r="T2">
@@ -4653,28 +4656,28 @@
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B3" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B3" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
       </c>
       <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>33</v>
@@ -4694,7 +4697,7 @@
       <c r="O3">
         <v>0.0</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="6">
         <v>31.25</v>
       </c>
       <c r="Q3">
@@ -4711,28 +4714,28 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B4" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B4" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
       </c>
       <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>33</v>
@@ -4740,7 +4743,7 @@
       <c r="K4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="6">
         <v>0.0</v>
       </c>
       <c r="M4">
@@ -4752,7 +4755,7 @@
       <c r="O4">
         <v>0.0</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="6">
         <v>31.25</v>
       </c>
       <c r="Q4">
@@ -4761,7 +4764,7 @@
       <c r="R4">
         <v>0.0</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4" s="6">
         <v>0.0</v>
       </c>
       <c r="T4">
@@ -4769,13 +4772,13 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B5" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B5" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -4783,16 +4786,16 @@
         <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>33</v>
@@ -4800,7 +4803,7 @@
       <c r="K5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="6">
         <v>20.75</v>
       </c>
       <c r="M5">
@@ -4821,7 +4824,7 @@
       <c r="R5">
         <v>0.0</v>
       </c>
-      <c r="S5" s="5">
+      <c r="S5" s="6">
         <v>20.75</v>
       </c>
       <c r="T5">
@@ -4829,25 +4832,25 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B6" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B6" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
         <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
       </c>
       <c r="I6" t="s">
         <v>40</v>
@@ -4856,12 +4859,12 @@
         <v>33</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="5">
+        <v>28</v>
+      </c>
+      <c r="L6" s="6">
         <v>18.75</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="6">
         <v>9.375</v>
       </c>
       <c r="N6">
@@ -4879,7 +4882,7 @@
       <c r="R6">
         <v>0.0</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S6" s="6">
         <v>18.75</v>
       </c>
       <c r="T6">
@@ -4887,25 +4890,25 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B7" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B7" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
         <v>40</v>
@@ -4928,7 +4931,7 @@
       <c r="O7">
         <v>0.0</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="6">
         <v>31.25</v>
       </c>
       <c r="Q7">
@@ -4945,25 +4948,25 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B8" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B8" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
         <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" t="s">
         <v>40</v>
@@ -4974,7 +4977,7 @@
       <c r="K8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="6">
         <v>0.0</v>
       </c>
       <c r="M8">
@@ -4986,7 +4989,7 @@
       <c r="O8">
         <v>0.0</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="6">
         <v>31.25</v>
       </c>
       <c r="Q8">
@@ -4995,7 +4998,7 @@
       <c r="R8">
         <v>0.0</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="6">
         <v>0.0</v>
       </c>
       <c r="T8">
@@ -5003,13 +5006,13 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="4">
+      <c r="A9" s="5">
         <f t="shared" si="1"/>
-        <v>43263</v>
-      </c>
-      <c r="B9" s="4">
+        <v>43264</v>
+      </c>
+      <c r="B9" s="5">
         <f t="shared" si="2"/>
-        <v>43628</v>
+        <v>43629</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -5017,13 +5020,13 @@
         <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" t="s">
         <v>40</v>
@@ -5034,7 +5037,7 @@
       <c r="K9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="6">
         <v>20.75</v>
       </c>
       <c r="M9">
@@ -5055,7 +5058,7 @@
       <c r="R9">
         <v>0.0</v>
       </c>
-      <c r="S9" s="5">
+      <c r="S9" s="6">
         <v>20.75</v>
       </c>
       <c r="T9">

</xml_diff>